<commit_message>
TText - removed `scopeObject`, because its REPRESENTATION is not sufficiently generic
</commit_message>
<xml_diff>
--- a/TText/_PGGM (Old Interfaces).xlsx
+++ b/TText/_PGGM (Old Interfaces).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="146">
   <si>
     <t>Customer</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Trx001</t>
   </si>
   <si>
-    <t>Car</t>
-  </si>
-  <si>
     <t>Car Insurance v0.1</t>
   </si>
   <si>
@@ -166,12 +163,6 @@
   </si>
   <si>
     <t>scopeDescr</t>
-  </si>
-  <si>
-    <t>scopeObject</t>
-  </si>
-  <si>
-    <t>ScopeObject</t>
   </si>
   <si>
     <t>ScopeDescr</t>
@@ -989,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,46 +995,37 @@
     <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1072,42 +1054,42 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>127</v>
-      </c>
       <c r="C1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1120,16 +1102,16 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1142,16 +1124,16 @@
         <v>Trx001</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1164,14 +1146,14 @@
         <v>Trx001</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1187,11 +1169,11 @@
         <v>0</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1204,13 +1186,13 @@
         <v>Trx001</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1223,10 +1205,10 @@
         <v>Trx001</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1239,10 +1221,10 @@
         <v>Trx001</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1295,36 +1277,36 @@
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1337,13 +1319,13 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1356,13 +1338,13 @@
         <v>Trx001</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1375,13 +1357,13 @@
         <v>Trx001</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1525,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1546,22 +1528,22 @@
   <sheetData>
     <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="F1" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1584,25 +1566,25 @@
     </row>
     <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1632,19 +1614,19 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1659,13 +1641,13 @@
         <v>Trx001</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -1679,16 +1661,16 @@
         <v>Trx001</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="7">
         <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1701,16 +1683,16 @@
         <v>Trx001</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="29">
         <v>5094</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1723,16 +1705,16 @@
         <v>Trx001</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1747,16 +1729,16 @@
         <v>Trx001</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="11">
         <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M8" s="7"/>
     </row>
@@ -1770,16 +1752,16 @@
         <v>Trx001</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1792,16 +1774,16 @@
         <v>Trx001</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1814,13 +1796,13 @@
         <v>Trx001</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
@@ -1833,16 +1815,16 @@
         <v>Trx001</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1855,16 +1837,16 @@
         <v>Trx001</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1877,16 +1859,16 @@
         <v>Trx001</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="11">
         <v>2002</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1899,19 +1881,19 @@
         <v>Trx001</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="11">
         <v>1234</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Var_Trx001_catalogusprijs</v>
@@ -1921,19 +1903,19 @@
         <v>Trx001</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="11">
         <v>22222</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Var_Trx001_polisbesluit</v>
@@ -1943,16 +1925,16 @@
         <v>Trx001</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Var_Trx001_conditionsurl</v>
@@ -1962,16 +1944,16 @@
         <v>Trx001</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Var_Trx001_eigenrisico</v>
@@ -1981,16 +1963,16 @@
         <v>Trx001</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Var_Trx001_CustomerSignature</v>
@@ -2000,13 +1982,13 @@
         <v>Trx001</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2085,13 +2067,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
@@ -2100,13 +2082,13 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -2119,10 +2101,10 @@
         <v>TNO</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2135,10 +2117,10 @@
         <v>PGGM</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="8"/>
@@ -2151,10 +2133,10 @@
         <v>RDW</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="8"/>
@@ -2167,10 +2149,10 @@
         <v>Overheid</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="8"/>
@@ -2191,13 +2173,13 @@
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -2206,13 +2188,13 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -2225,10 +2207,10 @@
         <v>person0</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2237,10 +2219,10 @@
         <v>person1</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2249,10 +2231,10 @@
         <v>person2</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2261,10 +2243,10 @@
         <v>person3</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2273,10 +2255,10 @@
         <v>person4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2285,10 +2267,10 @@
         <v>person5</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2311,45 +2293,45 @@
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="E20" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="F20" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="G20" s="24" t="s">
         <v>74</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="24" t="s">
         <v>78</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="G21" s="24" t="str">
         <f>$A21</f>
@@ -2362,17 +2344,17 @@
         <v>Acc_0</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" s="27" t="str">
         <f>IF(OR($B22="",$C22=""),"",$A11)</f>
         <v>person0</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2381,7 +2363,7 @@
         <v>Acc_1</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C23" s="14" t="str">
         <f>IF($B23="","","*****")</f>
@@ -2392,7 +2374,7 @@
         <v>person1</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23" s="14" t="str">
         <f>$A23</f>
@@ -2405,7 +2387,7 @@
         <v>Acc_2</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" s="14" t="str">
         <f t="shared" ref="C24:C31" si="4">IF($B24="","","*****")</f>
@@ -2416,7 +2398,7 @@
         <v>person2</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2425,7 +2407,7 @@
         <v>Acc_3</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C25" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2436,7 +2418,7 @@
         <v>person3</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2445,7 +2427,7 @@
         <v>Acc_4</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2462,7 +2444,7 @@
         <v>Acc_5</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" s="14" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
TText - simplified TParty implementation
</commit_message>
<xml_diff>
--- a/TText/_PGGM (Old Interfaces).xlsx
+++ b/TText/_PGGM (Old Interfaces).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
   <si>
     <t>Customer</t>
   </si>
@@ -114,21 +114,9 @@
     <t>Party that provides car insurance policies</t>
   </si>
   <si>
-    <t>Driver</t>
-  </si>
-  <si>
-    <t>Party that will be driving the (to be insured) car most regularly</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
     <t>drivers address</t>
   </si>
   <si>
-    <t>An automaton that is capable of computing variables/statements</t>
-  </si>
-  <si>
     <t>carinfo</t>
   </si>
   <si>
@@ -369,9 +357,6 @@
     <t>d.rijder@gmail.com</t>
   </si>
   <si>
-    <t>Acc_5</t>
-  </si>
-  <si>
     <t>[postcode]  [housenumber]</t>
   </si>
   <si>
@@ -420,15 +405,6 @@
     <t>[TParties]</t>
   </si>
   <si>
-    <t>tPartyDescr</t>
-  </si>
-  <si>
-    <t>tPartyName</t>
-  </si>
-  <si>
-    <t>tPartyScope</t>
-  </si>
-  <si>
     <t>tPartyAcc</t>
   </si>
   <si>
@@ -490,6 +466,9 @@
   </si>
   <si>
     <t>Het bepalen van het risico op ongevallen</t>
+  </si>
+  <si>
+    <t>ttDescr</t>
   </si>
 </sst>
 </file>
@@ -982,7 +961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -997,13 +976,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1011,10 +990,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1038,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,42 +1033,42 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1111,7 +1090,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1133,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1153,7 +1132,7 @@
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1173,59 +1152,47 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>SHR_Trx001_Driver</v>
+        <v>SHR_Trx001_PrevInsurer</v>
       </c>
       <c r="B7" s="21" t="str">
         <f>IF($C7="","",'#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>20</v>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>SHR_Trx001_PrevInsurer</v>
+        <v/>
       </c>
       <c r="B8" s="21" t="str">
         <f>IF($C8="","",'#Scopes'!$A$3)</f>
-        <v>Trx001</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>18</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>SHR_Trx001_Computer</v>
+        <v/>
       </c>
       <c r="B9" s="21" t="str">
         <f>IF($C9="","",'#Scopes'!$A$3)</f>
-        <v>Trx001</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>24</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
@@ -1277,36 +1244,36 @@
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1319,13 +1286,13 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1338,13 +1305,13 @@
         <v>Trx001</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1357,13 +1324,13 @@
         <v>Trx001</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1528,22 +1495,22 @@
   <sheetData>
     <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1566,25 +1533,25 @@
     </row>
     <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1614,19 +1581,19 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1647,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -1670,7 +1637,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1692,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1708,13 +1675,13 @@
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1738,7 +1705,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M8" s="7"/>
     </row>
@@ -1752,16 +1719,16 @@
         <v>Trx001</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1774,16 +1741,16 @@
         <v>Trx001</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1796,13 +1763,13 @@
         <v>Trx001</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
@@ -1815,16 +1782,16 @@
         <v>Trx001</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1837,16 +1804,16 @@
         <v>Trx001</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1859,7 +1826,7 @@
         <v>Trx001</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" s="11">
         <v>2002</v>
@@ -1868,7 +1835,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1881,7 +1848,7 @@
         <v>Trx001</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D15" s="11">
         <v>1234</v>
@@ -1890,7 +1857,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
@@ -1903,7 +1870,7 @@
         <v>Trx001</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D16" s="11">
         <v>22222</v>
@@ -1912,7 +1879,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1925,13 +1892,13 @@
         <v>Trx001</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1944,13 +1911,13 @@
         <v>Trx001</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1963,13 +1930,13 @@
         <v>Trx001</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1982,13 +1949,13 @@
         <v>Trx001</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2067,13 +2034,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
@@ -2082,13 +2049,13 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -2101,10 +2068,10 @@
         <v>TNO</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2120,7 +2087,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="8"/>
@@ -2136,7 +2103,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="8"/>
@@ -2149,10 +2116,10 @@
         <v>Overheid</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="8"/>
@@ -2173,13 +2140,13 @@
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -2188,13 +2155,13 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -2207,10 +2174,10 @@
         <v>person0</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2219,10 +2186,10 @@
         <v>person1</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2231,10 +2198,10 @@
         <v>person2</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2243,10 +2210,10 @@
         <v>person3</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2255,10 +2222,10 @@
         <v>person4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2267,10 +2234,10 @@
         <v>person5</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2293,45 +2260,45 @@
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="F20" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="G20" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G21" s="24" t="str">
         <f>$A21</f>
@@ -2344,17 +2311,17 @@
         <v>Acc_0</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D22" s="27" t="str">
         <f>IF(OR($B22="",$C22=""),"",$A11)</f>
         <v>person0</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2363,7 +2330,7 @@
         <v>Acc_1</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C23" s="14" t="str">
         <f>IF($B23="","","*****")</f>
@@ -2387,7 +2354,7 @@
         <v>Acc_2</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C24" s="14" t="str">
         <f t="shared" ref="C24:C31" si="4">IF($B24="","","*****")</f>
@@ -2407,7 +2374,7 @@
         <v>Acc_3</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C25" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2418,7 +2385,7 @@
         <v>person3</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2427,7 +2394,7 @@
         <v>Acc_4</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C26" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2444,7 +2411,7 @@
         <v>Acc_5</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C27" s="14" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
TText - further simplification and modularizations.
</commit_message>
<xml_diff>
--- a/TText/_PGGM (Old Interfaces).xlsx
+++ b/TText/_PGGM (Old Interfaces).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
@@ -309,12 +309,6 @@
     <t>polisadm@pggm.nl</t>
   </si>
   <si>
-    <t>Connie</t>
-  </si>
-  <si>
-    <t>Sument</t>
-  </si>
-  <si>
     <t>cs12345@gmail.com</t>
   </si>
   <si>
@@ -469,6 +463,12 @@
   </si>
   <si>
     <t>ttDescr</t>
+  </si>
+  <si>
+    <t>Connie-Sue</t>
+  </si>
+  <si>
+    <t>Menter</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1033,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>36</v>
@@ -1042,18 +1042,18 @@
         <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>1</v>
@@ -1090,7 +1090,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1112,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1244,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>36</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>1</v>
@@ -1286,13 +1286,13 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1305,13 +1305,13 @@
         <v>Trx001</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1324,13 +1324,13 @@
         <v>Trx001</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1551,7 +1551,7 @@
         <v>41</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1581,7 +1581,7 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>45</v>
@@ -1590,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -1637,7 +1637,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1659,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1681,7 +1681,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1705,7 +1705,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M8" s="7"/>
     </row>
@@ -1725,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1747,10 +1747,10 @@
         <v>8</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1791,7 +1791,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1813,7 +1813,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1835,7 +1835,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1857,7 +1857,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
@@ -1879,7 +1879,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1892,13 +1892,13 @@
         <v>Trx001</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1911,13 +1911,13 @@
         <v>Trx001</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1930,13 +1930,13 @@
         <v>Trx001</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1949,13 +1949,13 @@
         <v>Trx001</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2103,7 +2103,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="8"/>
@@ -2116,10 +2116,10 @@
         <v>Overheid</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="8"/>
@@ -2210,10 +2210,10 @@
         <v>person3</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2222,10 +2222,10 @@
         <v>person4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2234,10 +2234,10 @@
         <v>person5</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2374,7 +2374,7 @@
         <v>Acc_3</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2385,7 +2385,7 @@
         <v>person3</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2394,7 +2394,7 @@
         <v>Acc_4</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2411,7 +2411,7 @@
         <v>Acc_5</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" s="14" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
TText update - NOT backward compatible !!! TParty is NO LONGER a specialization but a Property. Also IDENT(Scope) is removed.
</commit_message>
<xml_diff>
--- a/TText/_PGGM (Old Interfaces).xlsx
+++ b/TText/_PGGM (Old Interfaces).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="138">
   <si>
     <t>Customer</t>
   </si>
@@ -393,9 +393,6 @@
     <t>Price of car [licenseplate], according to the catalogue of the manufacturer, in Euro.</t>
   </si>
   <si>
-    <t>TParty</t>
-  </si>
-  <si>
     <t>[TParties]</t>
   </si>
   <si>
@@ -408,9 +405,6 @@
     <t>[Concerns]</t>
   </si>
   <si>
-    <t>Concern</t>
-  </si>
-  <si>
     <t>Beslissing</t>
   </si>
   <si>
@@ -469,6 +463,9 @@
   </si>
   <si>
     <t>Menter</t>
+  </si>
+  <si>
+    <t>ttIsaTParty</t>
   </si>
 </sst>
 </file>
@@ -1015,210 +1012,254 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="14" customWidth="1"/>
-    <col min="4" max="4" width="64.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="14" customWidth="1"/>
+    <col min="5" max="5" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="24" t="str">
+        <f>IF($A2="","",$A2)</f>
+        <v>TText</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
-        <f>IF(OR($B3="",$C3=""),"",CONCATENATE("SHR_",$B3,"_",$C3))</f>
+        <f t="shared" ref="A3:A11" si="0">IF(OR($C3="",$D3=""),"",CONCATENATE("SHR_",$C3,"_",$D3))</f>
         <v>SHR_Trx001_Insurer</v>
       </c>
       <c r="B3" s="21" t="str">
-        <f>IF($C3="","",'#Scopes'!$A$3)</f>
+        <f>IF($A3="","",$A3)</f>
+        <v>SHR_Trx001_Insurer</v>
+      </c>
+      <c r="C3" s="21" t="str">
+        <f>IF($D3="","",'#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
-        <f t="shared" ref="A4:A11" si="0">IF(OR($B4="",$C4=""),"",CONCATENATE("SHR_",$B4,"_",$C4))</f>
+        <f t="shared" si="0"/>
         <v>SHR_Trx001_RDW</v>
       </c>
       <c r="B4" s="21" t="str">
-        <f>IF($C4="","",'#Scopes'!$A$3)</f>
+        <f t="shared" ref="B4:B11" si="1">IF($A4="","",$A4)</f>
+        <v>SHR_Trx001_RDW</v>
+      </c>
+      <c r="C4" s="21" t="str">
+        <f>IF($D4="","",'#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>SHR_Trx001_AP</v>
       </c>
       <c r="B5" s="21" t="str">
-        <f>IF($C5="","",'#Scopes'!$A$3)</f>
+        <f t="shared" si="1"/>
+        <v>SHR_Trx001_AP</v>
+      </c>
+      <c r="C5" s="21" t="str">
+        <f>IF($D5="","",'#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="str">
-        <f>IF(OR($B6="",$C6=""),"",CONCATENATE("SHR_",$B6,"_",$C6))</f>
+        <f t="shared" si="0"/>
         <v>SHR_Trx001_Customer</v>
       </c>
       <c r="B6" s="21" t="str">
-        <f>IF($C6="","",'#Scopes'!$A$3)</f>
+        <f t="shared" si="1"/>
+        <v>SHR_Trx001_Customer</v>
+      </c>
+      <c r="C6" s="21" t="str">
+        <f>IF($D6="","",'#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>SHR_Trx001_PrevInsurer</v>
       </c>
       <c r="B7" s="21" t="str">
-        <f>IF($C7="","",'#Scopes'!$A$3)</f>
+        <f t="shared" si="1"/>
+        <v>SHR_Trx001_PrevInsurer</v>
+      </c>
+      <c r="C7" s="21" t="str">
+        <f>IF($D7="","",'#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B8" s="21" t="str">
-        <f>IF($C8="","",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C8" s="21" t="str">
+        <f>IF($D8="","",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B9" s="21" t="str">
-        <f>IF($C9="","",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C9" s="21" t="str">
+        <f>IF($D9="","",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B10" s="21" t="str">
-        <f>IF($C10="","",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C10" s="21" t="str">
+        <f>IF($D10="","",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B11" s="21" t="str">
-        <f>IF($C11="","",'#Scopes'!$A$3)</f>
-        <v/>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="8"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="21" t="str">
+        <f>IF($D11="","",'#Scopes'!$A$3)</f>
+        <v/>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1229,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1285,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>36</v>
@@ -1261,7 +1302,7 @@
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>118</v>
+        <v>29</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>1</v>
@@ -1286,13 +1327,13 @@
         <v>Trx001</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1305,13 +1346,13 @@
         <v>Trx001</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1324,13 +1365,13 @@
         <v>Trx001</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1551,7 +1592,7 @@
         <v>41</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1593,7 +1634,7 @@
         <v>104</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1728,7 +1769,7 @@
         <v>99</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1750,7 +1791,7 @@
         <v>100</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1892,13 +1933,13 @@
         <v>Trx001</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1911,13 +1952,13 @@
         <v>Trx001</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1930,13 +1971,13 @@
         <v>Trx001</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1949,13 +1990,13 @@
         <v>Trx001</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2018,7 +2059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2222,10 +2263,10 @@
         <v>person4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TText - changes/cleanup for refactorization - Users will need to revise their TText_Module.adl (see: TText_ModuleExample.adl)
</commit_message>
<xml_diff>
--- a/TText/_PGGM (Old Interfaces).xlsx
+++ b/TText/_PGGM (Old Interfaces).xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="13800" windowHeight="5472" tabRatio="703" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
-    <sheet name="#TParties" sheetId="14" r:id="rId2"/>
-    <sheet name="#Concerns" sheetId="19" r:id="rId3"/>
-    <sheet name="#TTexts" sheetId="6" r:id="rId4"/>
-    <sheet name="SIAM" sheetId="18" r:id="rId5"/>
+    <sheet name="_#Scopes" sheetId="1" r:id="rId1"/>
+    <sheet name="_#TParties" sheetId="14" r:id="rId2"/>
+    <sheet name="_#Concerns" sheetId="19" r:id="rId3"/>
+    <sheet name="_#TTexts" sheetId="6" r:id="rId4"/>
+    <sheet name="__SIAM" sheetId="18" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -23,7 +23,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="G20" authorId="0">
+    <comment ref="G17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="137">
   <si>
     <t>Customer</t>
   </si>
@@ -180,9 +180,6 @@
     <t>TTPhrase</t>
   </si>
   <si>
-    <t>[Organization,]</t>
-  </si>
-  <si>
     <t>ttValue</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>[Role,]</t>
-  </si>
-  <si>
     <t>tinus.otto@tno.nl</t>
   </si>
   <si>
@@ -466,6 +460,9 @@
   </si>
   <si>
     <t>ttIsaTParty</t>
+  </si>
+  <si>
+    <t>Role</t>
   </si>
 </sst>
 </file>
@@ -959,7 +956,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,10 +1028,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>36</v>
@@ -1043,13 +1040,13 @@
         <v>37</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1070,10 +1067,10 @@
         <v>41</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1086,7 +1083,7 @@
         <v>SHR_Trx001_Insurer</v>
       </c>
       <c r="C3" s="21" t="str">
-        <f>IF($D3="","",'#Scopes'!$A$3)</f>
+        <f>IF($D3="","",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1099,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1112,7 +1109,7 @@
         <v>SHR_Trx001_RDW</v>
       </c>
       <c r="C4" s="21" t="str">
-        <f>IF($D4="","",'#Scopes'!$A$3)</f>
+        <f>IF($D4="","",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -1125,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1138,7 +1135,7 @@
         <v>SHR_Trx001_AP</v>
       </c>
       <c r="C5" s="21" t="str">
-        <f>IF($D5="","",'#Scopes'!$A$3)</f>
+        <f>IF($D5="","",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -1149,7 +1146,7 @@
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1162,7 +1159,7 @@
         <v>SHR_Trx001_Customer</v>
       </c>
       <c r="C6" s="21" t="str">
-        <f>IF($D6="","",'#Scopes'!$A$3)</f>
+        <f>IF($D6="","",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1173,7 +1170,7 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1186,7 +1183,7 @@
         <v>SHR_Trx001_PrevInsurer</v>
       </c>
       <c r="C7" s="21" t="str">
-        <f>IF($D7="","",'#Scopes'!$A$3)</f>
+        <f>IF($D7="","",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -1206,7 +1203,7 @@
         <v/>
       </c>
       <c r="C8" s="21" t="str">
-        <f>IF($D8="","",'#Scopes'!$A$3)</f>
+        <f>IF($D8="","",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
       <c r="D8" s="11"/>
@@ -1222,7 +1219,7 @@
         <v/>
       </c>
       <c r="C9" s="21" t="str">
-        <f>IF($D9="","",'#Scopes'!$A$3)</f>
+        <f>IF($D9="","",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
       <c r="E9" s="18"/>
@@ -1237,7 +1234,7 @@
         <v/>
       </c>
       <c r="C10" s="21" t="str">
-        <f>IF($D10="","",'#Scopes'!$A$3)</f>
+        <f>IF($D10="","",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
       <c r="D10" s="11"/>
@@ -1253,7 +1250,7 @@
         <v/>
       </c>
       <c r="C11" s="21" t="str">
-        <f>IF($D11="","",'#Scopes'!$A$3)</f>
+        <f>IF($D11="","",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
       <c r="D11" s="7"/>
@@ -1270,7 +1267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1285,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>36</v>
@@ -1323,17 +1320,17 @@
         <v>Conc_Trx001_Beslissing</v>
       </c>
       <c r="B3" s="15" t="str">
-        <f>IF(AND($E3="",$C3=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E3="",$C3=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1342,17 +1339,17 @@
         <v>Conc_Trx001_Customer Agreement</v>
       </c>
       <c r="B4" s="15" t="str">
-        <f>IF(AND($E4="",$C4=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E4="",$C4=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1361,17 +1358,17 @@
         <v>Conc_Trx001_Eigen Risico</v>
       </c>
       <c r="B5" s="15" t="str">
-        <f>IF(AND($E5="",$C5=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E5="",$C5=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1380,7 +1377,7 @@
         <v/>
       </c>
       <c r="B6" s="15" t="str">
-        <f>IF(AND($E6="",$C6=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E6="",$C6=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
       <c r="D6" s="8"/>
@@ -1391,7 +1388,7 @@
         <v/>
       </c>
       <c r="B7" s="15" t="str">
-        <f>IF(AND($E7="",$C7=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E7="",$C7=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
       <c r="D7" s="11"/>
@@ -1402,7 +1399,7 @@
         <v/>
       </c>
       <c r="B8" s="15" t="str">
-        <f>IF(AND($E8="",$C8=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E8="",$C8=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1412,7 +1409,7 @@
         <v/>
       </c>
       <c r="B9" s="15" t="str">
-        <f>IF(AND($E9="",$C9=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E9="",$C9=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1422,7 +1419,7 @@
         <v/>
       </c>
       <c r="B10" s="15" t="str">
-        <f>IF(AND($E10="",$C10=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E10="",$C10=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1432,7 +1429,7 @@
         <v/>
       </c>
       <c r="B11" s="15" t="str">
-        <f>IF(AND($E11="",$C11=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E11="",$C11=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1442,7 +1439,7 @@
         <v/>
       </c>
       <c r="B12" s="15" t="str">
-        <f>IF(AND($E12="",$C12=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E12="",$C12=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1452,7 +1449,7 @@
         <v/>
       </c>
       <c r="B13" s="15" t="str">
-        <f>IF(AND($E13="",$C13=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E13="",$C13=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1462,7 +1459,7 @@
         <v/>
       </c>
       <c r="B14" s="15" t="str">
-        <f>IF(AND($E14="",$C14=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E14="",$C14=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1472,7 +1469,7 @@
         <v/>
       </c>
       <c r="B15" s="15" t="str">
-        <f>IF(AND($E15="",$C15=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E15="",$C15=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1482,7 +1479,7 @@
         <v/>
       </c>
       <c r="B16" s="15" t="str">
-        <f>IF(AND($E16="",$C16=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E16="",$C16=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1492,7 +1489,7 @@
         <v/>
       </c>
       <c r="B17" s="15" t="str">
-        <f>IF(AND($E17="",$C17=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E17="",$C17=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1502,7 +1499,7 @@
         <v/>
       </c>
       <c r="B18" s="15" t="str">
-        <f>IF(AND($E18="",$C18=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($E18="",$C18=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -1545,7 +1542,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>38</v>
@@ -1583,7 +1580,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>40</v>
@@ -1592,7 +1589,7 @@
         <v>41</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1618,23 +1615,23 @@
         <v>Var_Trx001_licenseplate</v>
       </c>
       <c r="B3" s="15" t="str">
-        <f>IF(AND($F3="",$C3=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F3="",$C3=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1645,7 +1642,7 @@
         <v>Var_Trx001_mileage</v>
       </c>
       <c r="B4" s="15" t="str">
-        <f>IF(AND($F4="",$C4=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F4="",$C4=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1655,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K4" s="7"/>
     </row>
@@ -1665,7 +1662,7 @@
         <v>Var_Trx001_no-claim</v>
       </c>
       <c r="B5" s="15" t="str">
-        <f>IF(AND($F5="",$C5=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F5="",$C5=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1678,7 +1675,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1687,7 +1684,7 @@
         <v>Var_Trx001_date-of-birth</v>
       </c>
       <c r="B6" s="15" t="str">
-        <f>IF(AND($F6="",$C6=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F6="",$C6=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -1700,7 +1697,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1709,20 +1706,20 @@
         <v>Var_Trx001_postcode</v>
       </c>
       <c r="B7" s="15" t="str">
-        <f>IF(AND($F7="",$C7=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F7="",$C7=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1733,7 +1730,7 @@
         <v>Var_Trx001_housenumber</v>
       </c>
       <c r="B8" s="15" t="str">
-        <f>IF(AND($F8="",$C8=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F8="",$C8=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1746,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M8" s="7"/>
     </row>
@@ -1756,7 +1753,7 @@
         <v>Var_Trx001_drivers address</v>
       </c>
       <c r="B9" s="15" t="str">
-        <f>IF(AND($F9="",$C9=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F9="",$C9=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1766,10 +1763,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1778,7 +1775,7 @@
         <v>Var_Trx001_carinfo</v>
       </c>
       <c r="B10" s="15" t="str">
-        <f>IF(AND($F10="",$C10=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F10="",$C10=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1788,10 +1785,10 @@
         <v>8</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1800,7 +1797,7 @@
         <v>Var_Trx001_premium</v>
       </c>
       <c r="B11" s="15" t="str">
-        <f>IF(AND($F11="",$C11=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F11="",$C11=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1819,20 +1816,20 @@
         <v>Var_Trx001_merk</v>
       </c>
       <c r="B12" s="15" t="str">
-        <f>IF(AND($F12="",$C12=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F12="",$C12=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1841,20 +1838,20 @@
         <v>Var_Trx001_type</v>
       </c>
       <c r="B13" s="15" t="str">
-        <f>IF(AND($F13="",$C13=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F13="",$C13=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1863,7 +1860,7 @@
         <v>Var_Trx001_bouwjaar</v>
       </c>
       <c r="B14" s="15" t="str">
-        <f>IF(AND($F14="",$C14=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F14="",$C14=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -1876,7 +1873,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1885,7 +1882,7 @@
         <v>Var_Trx001_gewicht</v>
       </c>
       <c r="B15" s="15" t="str">
-        <f>IF(AND($F15="",$C15=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F15="",$C15=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -1898,7 +1895,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
@@ -1907,7 +1904,7 @@
         <v>Var_Trx001_catalogusprijs</v>
       </c>
       <c r="B16" s="15" t="str">
-        <f>IF(AND($F16="",$C16=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F16="",$C16=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -1920,7 +1917,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1929,17 +1926,17 @@
         <v>Var_Trx001_polisbesluit</v>
       </c>
       <c r="B17" s="15" t="str">
-        <f>IF(AND($F17="",$C17=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F17="",$C17=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1948,17 +1945,17 @@
         <v>Var_Trx001_conditionsurl</v>
       </c>
       <c r="B18" s="15" t="str">
-        <f>IF(AND($F18="",$C18=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F18="",$C18=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1967,17 +1964,17 @@
         <v>Var_Trx001_eigenrisico</v>
       </c>
       <c r="B19" s="15" t="str">
-        <f>IF(AND($F19="",$C19=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F19="",$C19=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1986,17 +1983,17 @@
         <v>Var_Trx001_CustomerSignature</v>
       </c>
       <c r="B20" s="15" t="str">
-        <f>IF(AND($F20="",$C20=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F20="",$C20=""),"",'_#Scopes'!$A$3)</f>
         <v>Trx001</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2005,7 +2002,7 @@
         <v/>
       </c>
       <c r="B21" s="15" t="str">
-        <f>IF(AND($F21="",$C21=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F21="",$C21=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -2015,7 +2012,7 @@
         <v/>
       </c>
       <c r="B22" s="15" t="str">
-        <f>IF(AND($F22="",$C22=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F22="",$C22=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -2025,7 +2022,7 @@
         <v/>
       </c>
       <c r="B23" s="15" t="str">
-        <f>IF(AND($F23="",$C23=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F23="",$C23=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -2035,7 +2032,7 @@
         <v/>
       </c>
       <c r="B24" s="15" t="str">
-        <f>IF(AND($F24="",$C24=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F24="",$C24=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -2045,7 +2042,7 @@
         <v/>
       </c>
       <c r="B25" s="15" t="str">
-        <f>IF(AND($F25="",$C25=""),"",'#Scopes'!$A$3)</f>
+        <f>IF(AND($F25="",$C25=""),"",'_#Scopes'!$A$3)</f>
         <v/>
       </c>
     </row>
@@ -2057,10 +2054,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2075,13 +2072,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
@@ -2090,13 +2087,13 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="24" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>54</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -2109,10 +2106,10 @@
         <v>TNO</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2121,14 +2118,14 @@
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="str">
-        <f t="shared" ref="A4:A8" si="0">IF($B4="","",$B4)</f>
+        <f t="shared" ref="A4:A7" si="0">IF($B4="","",$B4)</f>
         <v>PGGM</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="8"/>
@@ -2144,7 +2141,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="8"/>
@@ -2157,10 +2154,10 @@
         <v>Overheid</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="8"/>
@@ -2173,304 +2170,329 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="24" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="str">
+        <f>IF(OR($B10="",$C10=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v>person0</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="C10" s="14" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="str">
-        <f>IF(OR($B11="",$C11=""),"",CONCATENATE("person",ROW()-ROW($A$11)))</f>
-        <v>person0</v>
+        <f>IF(OR($B11="",$C11=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v>person1</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="str">
-        <f t="shared" ref="A12:A19" si="1">IF(OR($B12="",$C12=""),"",CONCATENATE("person",ROW()-ROW($A$11)))</f>
-        <v>person1</v>
+        <f>IF(OR($B12="",$C12=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v>person2</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>person2</v>
+        <f>IF(OR($B13="",$C13=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v>person3</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>person3</v>
+        <f>IF(OR($B14="",$C14=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v>person4</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>person4</v>
+        <f>IF(OR($B15="",$C15=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v>person5</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>person5</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f>IF(OR($B16="",$C16=""),"",CONCATENATE("person",ROW()-ROW($A$10)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="24" t="str">
+        <f>$A18</f>
+        <v>Account</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="str">
+        <f>IF(OR($B19="",$C19=""),"",CONCATENATE("Acc_",ROW()-ROW($A$19)))</f>
+        <v>Acc_0</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="27" t="str">
+        <f>IF(OR($B19="",$C19=""),"",$A10)</f>
+        <v>person0</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="str">
+        <f t="shared" ref="A20:A28" si="1">IF(OR($B20="",$C20=""),"",CONCATENATE("Acc_",ROW()-ROW($A$19)))</f>
+        <v>Acc_1</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="14" t="str">
+        <f>IF($B20="","","*****")</f>
+        <v>*****</v>
+      </c>
+      <c r="D20" s="27" t="str">
+        <f>IF(OR($B20="",$C20=""),"",$A11)</f>
+        <v>person1</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="14" t="str">
+        <f>$A20</f>
+        <v>Acc_1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="24" t="str">
-        <f>$A21</f>
-        <v>Account</v>
+        <v>Acc_2</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="14" t="str">
+        <f t="shared" ref="C21:C28" si="2">IF($B21="","","*****")</f>
+        <v>*****</v>
+      </c>
+      <c r="D21" s="27" t="str">
+        <f>IF(OR($B21="",$C21=""),"",$A12)</f>
+        <v>person2</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="str">
-        <f>IF(OR($B22="",$C22=""),"",CONCATENATE("Acc_",ROW()-ROW($A$22)))</f>
-        <v>Acc_0</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>76</v>
+        <f t="shared" si="1"/>
+        <v>Acc_3</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>*****</v>
       </c>
       <c r="D22" s="27" t="str">
-        <f>IF(OR($B22="",$C22=""),"",$A11)</f>
-        <v>person0</v>
+        <f>IF(OR($B22="",$C22=""),"",$A13)</f>
+        <v>person3</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="str">
-        <f t="shared" ref="A23:A31" si="2">IF(OR($B23="",$C23=""),"",CONCATENATE("Acc_",ROW()-ROW($A$22)))</f>
-        <v>Acc_1</v>
+        <f t="shared" si="1"/>
+        <v>Acc_4</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" s="14" t="str">
-        <f>IF($B23="","","*****")</f>
+        <f t="shared" si="2"/>
         <v>*****</v>
       </c>
       <c r="D23" s="27" t="str">
-        <f t="shared" ref="D23:D31" si="3">IF(OR($B23="",$C23=""),"",$A12)</f>
-        <v>person1</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="14" t="str">
-        <f>$A23</f>
-        <v>Acc_1</v>
+        <f>IF(OR($B23="",$C23=""),"",$A14)</f>
+        <v>person4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>Acc_5</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_2</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="14" t="str">
-        <f t="shared" ref="C24:C31" si="4">IF($B24="","","*****")</f>
         <v>*****</v>
       </c>
       <c r="D24" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v>person2</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>8</v>
+        <f>IF(OR($B24="",$C24=""),"",$A15)</f>
+        <v>person5</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_3</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v>*****</v>
+        <v/>
       </c>
       <c r="D25" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v>person3</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>87</v>
+        <f>IF(OR($B25="",$C25=""),"",#REF!)</f>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_4</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v>*****</v>
+        <v/>
       </c>
       <c r="D26" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v>person4</v>
+        <f>IF(OR($B26="",$C26=""),"",#REF!)</f>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C27" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>Acc_5</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v>*****</v>
+        <v/>
       </c>
       <c r="D27" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v>person5</v>
+        <f t="shared" ref="D27:D28" si="3">IF(OR($B27="",$C27=""),"",$A16)</f>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C28" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="14" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D28" s="27" t="str">
@@ -2478,67 +2500,24 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="D29" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C30" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="D30" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C31" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="D31" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C23:C31">
+  <conditionalFormatting sqref="C20:C28">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"*****"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C31">
+  <conditionalFormatting sqref="C20:C28">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C23))=0</formula>
+      <formula>LEN(TRIM(C20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1"/>
-    <hyperlink ref="B25" r:id="rId2"/>
-    <hyperlink ref="B23" r:id="rId3"/>
-    <hyperlink ref="B24" r:id="rId4"/>
-    <hyperlink ref="B26" r:id="rId5"/>
-    <hyperlink ref="B27" r:id="rId6"/>
+    <hyperlink ref="B19" r:id="rId1"/>
+    <hyperlink ref="B22" r:id="rId2"/>
+    <hyperlink ref="B20" r:id="rId3"/>
+    <hyperlink ref="B21" r:id="rId4"/>
+    <hyperlink ref="B23" r:id="rId5"/>
+    <hyperlink ref="B24" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>

</xml_diff>